<commit_message>
Change values in the excel sheet
</commit_message>
<xml_diff>
--- a/data/proportions_obs_pred_data.xlsx
+++ b/data/proportions_obs_pred_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ihsan/Documents/valascotraceR/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4471707-3ED4-6746-BF02-BDF086C24717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77923DEC-4277-CF4B-AF5E-FD5BB60D605F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{4CDB6406-8499-4A71-A0AD-A91DC68DA5E4}"/>
   </bookViews>
@@ -415,7 +415,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -479,7 +479,7 @@
         <v>0.26</v>
       </c>
       <c r="D4" s="1">
-        <v>0.48</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -493,7 +493,7 @@
         <v>0.44</v>
       </c>
       <c r="D5" s="1">
-        <v>0.92</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -507,7 +507,7 @@
         <v>0.49</v>
       </c>
       <c r="D6" s="1">
-        <v>0.92</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -521,7 +521,7 @@
         <v>0.52</v>
       </c>
       <c r="D7" s="1">
-        <v>0.92</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -535,7 +535,7 @@
         <v>0.61</v>
       </c>
       <c r="D8" s="1">
-        <v>0.92</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -549,7 +549,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="1">
-        <v>0.92</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -605,7 +605,7 @@
         <v>0.03</v>
       </c>
       <c r="D13" s="1">
-        <v>0.52</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -619,7 +619,7 @@
         <v>0.11</v>
       </c>
       <c r="D14" s="1">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -633,7 +633,7 @@
         <v>0.19</v>
       </c>
       <c r="D15" s="1">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -647,7 +647,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="D16" s="1">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -661,7 +661,7 @@
         <v>0.4</v>
       </c>
       <c r="D17" s="1">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -675,7 +675,7 @@
         <v>0.96</v>
       </c>
       <c r="D18" s="1">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -689,7 +689,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="1">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update values in the spreadsheet
</commit_message>
<xml_diff>
--- a/data/proportions_obs_pred_data.xlsx
+++ b/data/proportions_obs_pred_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ihsan/Documents/valascotraceR/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77923DEC-4277-CF4B-AF5E-FD5BB60D605F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34530CEA-435C-E645-B2EF-1975F50BCD1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{4CDB6406-8499-4A71-A0AD-A91DC68DA5E4}"/>
   </bookViews>
@@ -415,7 +415,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -479,7 +479,7 @@
         <v>0.26</v>
       </c>
       <c r="D4" s="1">
-        <v>0.84</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -493,7 +493,7 @@
         <v>0.44</v>
       </c>
       <c r="D5" s="1">
-        <v>0.96</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -507,7 +507,7 @@
         <v>0.49</v>
       </c>
       <c r="D6" s="1">
-        <v>0.96</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -521,7 +521,7 @@
         <v>0.52</v>
       </c>
       <c r="D7" s="1">
-        <v>0.96</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -535,7 +535,7 @@
         <v>0.61</v>
       </c>
       <c r="D8" s="1">
-        <v>0.96</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -549,7 +549,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="1">
-        <v>0.96</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -605,7 +605,7 @@
         <v>0.03</v>
       </c>
       <c r="D13" s="1">
-        <v>0.68</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -619,7 +619,7 @@
         <v>0.11</v>
       </c>
       <c r="D14" s="1">
-        <v>0.8</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -633,7 +633,7 @@
         <v>0.19</v>
       </c>
       <c r="D15" s="1">
-        <v>1</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -647,7 +647,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="D16" s="1">
-        <v>1</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -661,7 +661,7 @@
         <v>0.4</v>
       </c>
       <c r="D17" s="1">
-        <v>1</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -675,7 +675,7 @@
         <v>0.96</v>
       </c>
       <c r="D18" s="1">
-        <v>1</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -689,7 +689,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="1">
-        <v>1</v>
+        <v>0.52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update prediction values after running the model 20 times
</commit_message>
<xml_diff>
--- a/data/proportions_obs_pred_data.xlsx
+++ b/data/proportions_obs_pred_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ihsan/Documents/valascotraceR/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34530CEA-435C-E645-B2EF-1975F50BCD1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7975E9FE-445F-3842-8083-40921F4418C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{4CDB6406-8499-4A71-A0AD-A91DC68DA5E4}"/>
   </bookViews>
@@ -415,7 +415,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -605,7 +605,7 @@
         <v>0.03</v>
       </c>
       <c r="D13" s="1">
-        <v>0.16</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -619,7 +619,7 @@
         <v>0.11</v>
       </c>
       <c r="D14" s="1">
-        <v>0.24</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -633,7 +633,7 @@
         <v>0.19</v>
       </c>
       <c r="D15" s="1">
-        <v>0.44</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -647,7 +647,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="D16" s="1">
-        <v>0.44</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -661,7 +661,7 @@
         <v>0.4</v>
       </c>
       <c r="D17" s="1">
-        <v>0.52</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -675,7 +675,7 @@
         <v>0.96</v>
       </c>
       <c r="D18" s="1">
-        <v>0.52</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -689,7 +689,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="1">
-        <v>0.52</v>
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>